<commit_message>
Print first try of print scissors.
</commit_message>
<xml_diff>
--- a/Picture Sources/Pictures.xlsx
+++ b/Picture Sources/Pictures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\XJTLU\Lessons\Year 2 Semester 1\EEE101\Assessment 2\Picture Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8841602-A6A6-457B-8A67-4A57FFD7B136}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D233A9F-8542-468B-BD68-135B821CE770}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
   </bookViews>
@@ -43,12 +43,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,8 +71,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -383,13 +392,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69BD16-3C5A-420A-B0AB-1B3565514C51}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the size of characters(normal and mini).
</commit_message>
<xml_diff>
--- a/Picture Sources/Pictures.xlsx
+++ b/Picture Sources/Pictures.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\XJTLU\Lessons\Year 2 Semester 1\EEE101\Assessment 2\Picture Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D233A9F-8542-468B-BD68-135B821CE770}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB7A80-F31E-4DA8-98A1-20F8B3D87D34}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" activeTab="2" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rock" sheetId="2" r:id="rId1"/>
+    <sheet name="Scissors(normal)" sheetId="1" r:id="rId2"/>
+    <sheet name="Scissors(mini)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -391,8 +393,498 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8C43F3-9F45-4C74-B114-C4915FE4FC66}">
+  <dimension ref="A1:U26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69BD16-3C5A-420A-B0AB-1B3565514C51}">
   <dimension ref="A1:U26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21997B2-A10C-4483-A535-750D7C35FC23}">
+  <dimension ref="A1:AM26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,156 +966,125 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="S4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM17" s="1"/>
+    </row>
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Add mini characters pictures in the welcome UI.
</commit_message>
<xml_diff>
--- a/Picture Sources/Pictures.xlsx
+++ b/Picture Sources/Pictures.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\XJTLU\Lessons\Year 2 Semester 1\EEE101\Assessment 2\Picture Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267F1D9A-F3ED-460A-8990-ACB9658E105D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E636B438-53B9-4C9B-8512-868A1EF0725F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" activeTab="2" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rock" sheetId="2" r:id="rId1"/>
-    <sheet name="Scissors(normal)" sheetId="1" r:id="rId2"/>
-    <sheet name="Scissors(mini)" sheetId="3" r:id="rId3"/>
+    <sheet name="Rock(normal)" sheetId="2" r:id="rId1"/>
+    <sheet name="Rock(mini) (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Scissors(normal)" sheetId="1" r:id="rId3"/>
+    <sheet name="Scissors(mini)" sheetId="3" r:id="rId4"/>
+    <sheet name="Paper(normal)" sheetId="5" r:id="rId5"/>
+    <sheet name="Paper(mini)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -394,7 +397,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8C43F3-9F45-4C74-B114-C4915FE4FC66}">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:BM26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="BM19" s="1"/>
+    </row>
+    <row r="20" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6E6898-1179-4608-84BD-CF1A3C431239}">
+  <dimension ref="A1:BM26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -476,401 +729,134 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="S4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="D5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BM19" s="1"/>
+    </row>
+    <row r="20" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69BD16-3C5A-420A-B0AB-1B3565514C51}">
-  <dimension ref="A1:U26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="M1">
-        <v>11</v>
-      </c>
-      <c r="N1">
-        <v>12</v>
-      </c>
-      <c r="O1">
-        <v>13</v>
-      </c>
-      <c r="P1">
-        <v>14</v>
-      </c>
-      <c r="Q1">
-        <v>15</v>
-      </c>
-      <c r="R1">
-        <v>16</v>
-      </c>
-      <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
-        <v>18</v>
-      </c>
-      <c r="U1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="R21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -883,12 +869,244 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69BD16-3C5A-420A-B0AB-1B3565514C51}">
+  <dimension ref="A1:AC26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AM17" sqref="AM17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21997B2-A10C-4483-A535-750D7C35FC23}">
   <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1097,4 +1315,517 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F1B7A4-8476-40C9-AA12-DBD498A9873A}">
+  <dimension ref="A1:AM26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="AM17" s="1"/>
+    </row>
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C0E9F3-04EB-49D5-B277-C751DF6C0BAF}">
+  <dimension ref="A1:AM26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="AM17" s="1"/>
+    </row>
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Repair the bug of current winner wrong when the user and computer are same with rock and scissors.
</commit_message>
<xml_diff>
--- a/Picture Sources/Pictures.xlsx
+++ b/Picture Sources/Pictures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\XJTLU\Lessons\Year 2 Semester 1\EEE101\Assessment 2\Picture Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E636B438-53B9-4C9B-8512-868A1EF0725F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0681FD-5F42-4D31-8542-0C64C67B70B3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" activeTab="4" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Rock(normal)" sheetId="2" r:id="rId1"/>
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8C43F3-9F45-4C74-B114-C4915FE4FC66}">
   <dimension ref="A1:BM26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -872,9 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69BD16-3C5A-420A-B0AB-1B3565514C51}">
   <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AM17" sqref="AM17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1321,7 +1319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F1B7A4-8476-40C9-AA12-DBD498A9873A}">
   <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Change the picture of rock and paper characters.
</commit_message>
<xml_diff>
--- a/Picture Sources/Pictures.xlsx
+++ b/Picture Sources/Pictures.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\XJTLU\Lessons\Year 2 Semester 1\EEE101\Assessment 2\Picture Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0681FD-5F42-4D31-8542-0C64C67B70B3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6222B288-E443-44EF-A02A-C001225603B4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" activeTab="4" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{9741BEE1-7884-4E5D-89E6-0A43CC52F8E3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rock(normal)" sheetId="2" r:id="rId1"/>
-    <sheet name="Rock(mini) (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Rock(normal)" sheetId="5" r:id="rId1"/>
+    <sheet name="Rock(mini)" sheetId="6" r:id="rId2"/>
     <sheet name="Scissors(normal)" sheetId="1" r:id="rId3"/>
     <sheet name="Scissors(mini)" sheetId="3" r:id="rId4"/>
-    <sheet name="Paper(normal)" sheetId="5" r:id="rId5"/>
-    <sheet name="Paper(mini)" sheetId="6" r:id="rId6"/>
+    <sheet name="Paper(normal)" sheetId="7" r:id="rId5"/>
+    <sheet name="Paper(mini)" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,6 +27,19 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="2">
+  <si>
+    <t>~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>|</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -76,12 +89,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,14 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8C43F3-9F45-4C74-B114-C4915FE4FC66}">
-  <dimension ref="A1:BM26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F1B7A4-8476-40C9-AA12-DBD498A9873A}">
+  <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -465,63 +481,66 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -532,25 +551,42 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -560,80 +596,95 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM17" s="1"/>
+    </row>
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="BM19" s="1"/>
-    </row>
-    <row r="20" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -646,14 +697,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6E6898-1179-4608-84BD-CF1A3C431239}">
-  <dimension ref="A1:BM26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C0E9F3-04EB-49D5-B277-C751DF6C0BAF}">
+  <dimension ref="A1:AM26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -715,148 +766,153 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB13" s="1"/>
+    </row>
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM17" s="1"/>
+    </row>
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="BM19" s="1"/>
-    </row>
-    <row r="20" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1316,14 +1372,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F1B7A4-8476-40C9-AA12-DBD498A9873A}">
-  <dimension ref="A1:AM26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D636EE-5CCD-44E7-A980-CA48387942B7}">
+  <dimension ref="A1:AK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -1349,74 +1405,162 @@
         <v>7</v>
       </c>
       <c r="J1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
-        <v>18</v>
-      </c>
-      <c r="U1">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="1"/>
+      <c r="M5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1424,10 +1568,24 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1437,13 +1595,25 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1452,14 +1622,25 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1468,14 +1649,25 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1484,12 +1676,24 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1499,12 +1703,26 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1512,86 +1730,363 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="1"/>
+      <c r="M13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="Z13" s="1"/>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="AM17" s="1"/>
-    </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="AK17" s="1"/>
+    </row>
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+    </row>
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1601,14 +2096,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C0E9F3-04EB-49D5-B277-C751DF6C0BAF}">
-  <dimension ref="A1:AM26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B614C8-7B3A-439C-834A-2C36FB985D2A}">
+  <dimension ref="A1:AK26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -1634,192 +2129,582 @@
         <v>7</v>
       </c>
       <c r="J1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="R1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S1">
-        <v>17</v>
-      </c>
-      <c r="T1">
-        <v>18</v>
-      </c>
-      <c r="U1">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="AM17" s="1"/>
-    </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="AK17" s="1"/>
+    </row>
+    <row r="18" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+    </row>
+    <row r="24" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>